<commit_message>
rolling window torch Dataset
</commit_message>
<xml_diff>
--- a/paper/my_writing/LiteReview/LiteReview_table.xlsx
+++ b/paper/my_writing/LiteReview/LiteReview_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0ngoing\thesis\repo\paper\my_writing\LiteReview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20739E0-CA21-407F-959A-EDEC5C1A10ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E694A5AA-A654-4688-8100-CF6FEE7F408E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="2430" windowWidth="8370" windowHeight="11835" firstSheet="1" activeTab="3" xr2:uid="{9A42303F-D228-42FB-A5BE-46881AB9C9FE}"/>
+    <workbookView xWindow="14715" yWindow="2430" windowWidth="8370" windowHeight="11835" firstSheet="1" activeTab="1" xr2:uid="{9A42303F-D228-42FB-A5BE-46881AB9C9FE}"/>
   </bookViews>
   <sheets>
     <sheet name="EPS Forecasting" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>Name(year)</t>
     <phoneticPr fontId="1"/>
@@ -466,6 +466,90 @@
   </si>
   <si>
     <t>本論文は，経営者予想に関する日米の研究をサーベイし，わが国における経営者予想研究の今後の課題を明らかにしている。なお本論文では，「経営者予想の資本市場における有用性」，「経営者予想の特性」，「経営者予想と他の予想の比較」の三点についてサーベイ結果をまとめている。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Forecast combinations of computational intelligence and linear
+models for the NN5 time series forecasting competition</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Multilayer Feedforward Networks are
+Universal Approximators</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Hornik (1989)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Neural Networks</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Hill et al. (1994a)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Artificial neural network models for forecasting and decision
+making</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Advances in forecasting with neural networks? Empirical evidence
+from the NN3 competition on time series prediction</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Crone et al. (2011)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Andrawis et al. (2011)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Hewamalage et al. (2011)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Recurrent Neural Networks for Time Series Forecasting:
+Current status and future directions</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NNは万能じゃないって言ってる。(季節性がある場合はいい)、もし自分の研究でANNが負けたらこれを引用して、アンチANNの方向でいこう。</t>
+    <rPh sb="3" eb="5">
+      <t>バンノウ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t>キセツセイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ケンキュウ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>マ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>インヨウ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ホウコウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1066,61 +1150,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3199158E-ED12-4C87-BFD6-72B9C0C6A161}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="11.125" style="1" customWidth="1"/>
-    <col min="3" max="13" width="30.625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col min="1" max="3" width="11.125" style="1" customWidth="1"/>
+    <col min="4" max="14" width="30.625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="131.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="150" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="225" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="225" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="187.5" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF1F84C-DD42-43C4-87BD-4B408B5D4395}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>